<commit_message>
Updated failed tests remedies.
</commit_message>
<xml_diff>
--- a/Dev/Server Tests Setup/failed spec remedies.xlsx
+++ b/Dev/Server Tests Setup/failed spec remedies.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\7232_Clone_5\Dev\Server Tests Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67867ACA-CC13-4A5F-89AB-D0BFBC9406CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAF4E90-9175-42E6-9F84-BA28A3D4F825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A2C2CC-61DF-41CE-BC13-38F583871B88}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
   <si>
     <t xml:space="preserve">SimpleWorkflowAssigningTo100RecordsExecutingAgainstTheServer </t>
   </si>
@@ -85,6 +85,15 @@
   <si>
     <t>Copy "c494711c-c6a4-44d5-abb9-c0339cd88bae\TestForSearchSpecs.test" folder in Programdata\Warewolf\Tests directory
 then Restart server and run test</t>
+  </si>
+  <si>
+    <t>SendingErrorInErrorVariableAndCallingWebservice</t>
+  </si>
+  <si>
+    <t>Connection with credentials "WarewolfAdmin" and W@rEw0lf@dm1n fails on "tst-ci-remote:3142" server and returns "(401) Unauthorized" error</t>
+  </si>
+  <si>
+    <t>Credentials on tst-ci-remote:3142 fails, need to correct the credentails (to be checked at tst-ci-remote:3142)</t>
   </si>
 </sst>
 </file>
@@ -451,7 +460,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,6 +562,17 @@
         <v>15</v>
       </c>
     </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added secureSettings in app.config Update Readme and failed spec remedies.xlsx to pass tests
</commit_message>
<xml_diff>
--- a/Dev/Server Tests Setup/failed spec remedies.xlsx
+++ b/Dev/Server Tests Setup/failed spec remedies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\7232_Clone_5\Dev\Server Tests Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAF4E90-9175-42E6-9F84-BA28A3D4F825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70142DD7-41F9-4719-8FAD-FA9695B1A57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A2C2CC-61DF-41CE-BC13-38F583871B88}"/>
   </bookViews>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
7427-Fixed the issues to pass failed tests in Dev2.Integration.Tests:
Change_sql_source_verify_Empty_Inputs - Moq Source setup
Added missing workflow - WorkflowWithNoStartNodeConnected.xml
Cleaup workflows
updated failed spec remedies for Dev2.Integration.Tests failed tests remedies
Replaced WebClient with HttpClient to fix authentication errors expecting default credentials
</commit_message>
<xml_diff>
--- a/Dev/Server Tests Setup/failed spec remedies.xlsx
+++ b/Dev/Server Tests Setup/failed spec remedies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\7232_Clone_5\Dev\Server Tests Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70142DD7-41F9-4719-8FAD-FA9695B1A57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97D18B-FE9F-4ED1-915B-4238AC70EF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A2C2CC-61DF-41CE-BC13-38F583871B88}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t xml:space="preserve">SimpleWorkflowAssigningTo100RecordsExecutingAgainstTheServer </t>
   </si>
@@ -94,6 +94,24 @@
   </si>
   <si>
     <t>Credentials on tst-ci-remote:3142 fails, need to correct the credentails (to be checked at tst-ci-remote:3142)</t>
+  </si>
+  <si>
+    <t>Dev2.Integration.Tests</t>
+  </si>
+  <si>
+    <t>Add_A_New_InputOnSqlProcedure_Expect_New_IS_InputAdded</t>
+  </si>
+  <si>
+    <t>copy resources, restart server, run again</t>
+  </si>
+  <si>
+    <t>Change_sql_source_verify_Empty_Inputs</t>
+  </si>
+  <si>
+    <t>ExecutionWithNoStartNode_ExpectedInvalidValidResult</t>
+  </si>
+  <si>
+    <t>copy file WorkflowWithNoStartNodeConnected.xml in Resources\Acceptance Testing Resources directory, restart server , run again</t>
   </si>
 </sst>
 </file>
@@ -457,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A839365-65E0-45F8-9697-64BA7363FDB8}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,6 +607,35 @@
         <v>8</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
7427-Updated failed spec remedies.xlsx to include remedies to pass failed tests in Dev2.Integration.Tests which has certain dependencies
</commit_message>
<xml_diff>
--- a/Dev/Server Tests Setup/failed spec remedies.xlsx
+++ b/Dev/Server Tests Setup/failed spec remedies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\7232_Clone_5\Dev\Server Tests Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA97D18B-FE9F-4ED1-915B-4238AC70EF05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C02C2D3-353E-4792-9E8C-7EACDFC960D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A2C2CC-61DF-41CE-BC13-38F583871B88}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
7432 - Updated tests and necessary envrionment setup to pass failed tests
Run_a_workflow_to_test_server_refresh - updated as per latest behaviour or resource cache
ExecuteRequest- WebClient is replaced with HttpClient
Resource cleanup done
</commit_message>
<xml_diff>
--- a/Dev/Server Tests Setup/failed spec remedies.xlsx
+++ b/Dev/Server Tests Setup/failed spec remedies.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\7232_Clone_5\Dev\Server Tests Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C02C2D3-353E-4792-9E8C-7EACDFC960D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6FFAF3-C1DC-417C-B590-5C57DC4C9C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A2C2CC-61DF-41CE-BC13-38F583871B88}"/>
   </bookViews>
@@ -478,7 +478,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
EsbHub updated to fix AddItemMessage - exception - object disposed Server Test Setup updated - to copy necessary resources and settings used by Dev2.Activitites.Specs
</commit_message>
<xml_diff>
--- a/Dev/Server Tests Setup/failed spec remedies.xlsx
+++ b/Dev/Server Tests Setup/failed spec remedies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Live\Warewolf\7232_Clone_5\Dev\Server Tests Setup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6FFAF3-C1DC-417C-B590-5C57DC4C9C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D42A79-C364-4E07-A204-9DB0C66E85BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{58A2C2CC-61DF-41CE-BC13-38F583871B88}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t xml:space="preserve">SimpleWorkflowAssigningTo100RecordsExecutingAgainstTheServer </t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>copy file WorkflowWithNoStartNodeConnected.xml in Resources\Acceptance Testing Resources directory, restart server , run again</t>
+  </si>
+  <si>
+    <t>Copy secure.config (found at the "ResumingAWorkflowWithAnInvalidUserReturnsAuthenticationError config" directory) file in the Directory "%Programdata%\Warewolf\Server Settings"</t>
   </si>
 </sst>
 </file>
@@ -477,8 +480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A839365-65E0-45F8-9697-64BA7363FDB8}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -558,7 +561,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">

</xml_diff>